<commit_message>
CONCEPTOS DE V &V EN DICCIONARIO
</commit_message>
<xml_diff>
--- a/Diccionario Acronimos  y Abreviaciones .xlsx
+++ b/Diccionario Acronimos  y Abreviaciones .xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Diccionario" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Acronimo</t>
   </si>
@@ -71,20 +71,147 @@
     <t>Manual de instalación</t>
   </si>
   <si>
-    <t>Documento que la informacion necesaria para garantizar la instalación y correcto funcionamiento del software</t>
-  </si>
-  <si>
     <t>Resultados de pruebas</t>
   </si>
   <si>
     <t>Documento que contiene los resultados de las diferentes pruebas realizadas al software (parcial o total)</t>
+  </si>
+  <si>
+    <t>Verificar</t>
+  </si>
+  <si>
+    <t>"Comprobar o examinar la verdad de algo [RAE], por  ejemplo: revisar que  un  requerimiento ha sido implementado" [IRONWORKS]</t>
+  </si>
+  <si>
+    <t>Comprobación de un conjunto de datos para determinar si su valor se halla dentro de unos límites de fiabilidad [VOX]" [IRONWORKS]</t>
+  </si>
+  <si>
+    <t>comprobar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Análisis de riesgos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">proceso de evaluar riesgos identificados para estimar su impacto y probabilidad de ocurrencia. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aseguramiento de la calidad (QA) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Caso de prueba </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Control de calidad (QC) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Driver </t>
+  </si>
+  <si>
+    <t xml:space="preserve">componente software o herramienta de prueba que reemplaza un componente que se encarga del control y/o de la llamada a un componente o sistema. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informe de incidencias de pruebas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Informe de resumen de pruebas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan de pruebas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prototipo: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pruebas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Riesgos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">factor que puede resultar en consecuencias negativas o positivas en el futuro. Normalmente se expresa en términos de impacto y probabilidad. </t>
+  </si>
+  <si>
+    <t>Documento que la información necesaria para garantizar la instalación y correcto funcionamiento del software</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conjunto de actividades diceñadas para asegurar que el proceso de desarrollo y/o mantenimiento es adecuado para que el sistema cumpla sus objetivos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conjunto de valores de entrada, precondiciones de ejecucióńn, resultados esperados y post condiciones de ejecucióńn desarrolladas para un objetivo o condición de prueba particular, tal como probar un determinado camino de un programa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">conjunto de actividades diceñadas para evaluar el producto de trabajo ya desarrollado </t>
+  </si>
+  <si>
+    <t xml:space="preserve">documento que recoge cualquier evento ocurrido durante el proceso de pruebas que requiera de investigacióńn y resolucióńn. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">documento que resume las actividades y resultados de las pruebas. Tambiéńn contiene la evaluacióńn de los elementos de prueba correspondientes. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peer reviews (Revisióńn entre pares) </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">las revisiones entre pares es un método de verificacióńn importante y eficaz implementado vía inspecciones, revisiones técnicas, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">walkthrough </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ArialMT"/>
+      </rPr>
+      <t xml:space="preserve">u otros métodos de revisión entre compañeros. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">documento que describe el alcance, el enfoque a seguir, los recursos a asignar y la planificacióńn de las actividades de pruebas. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">borrador de un producto potencial o de una parte del mismo, una simulacióńn de los requisitos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">actividad en la cual un sistema, o uno de sus componentes, se ejecutan en circunstancias previamente especificadas, se observan los resultados, se registran y se realiza una evaluacióńn de mismos. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISO </t>
+  </si>
+  <si>
+    <t>(International Organization for Standarization): Organización Internacional para la Estandarización.</t>
+  </si>
+  <si>
+    <t>Aseguramiento de calidad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA (Quality Assurance) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">QC (Quality Control): </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Control de calidad </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SVVP (Software Verification and Validation Plan) </t>
+  </si>
+  <si>
+    <t>Plan de Verificación y Validación.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -116,6 +243,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ArialMT"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -134,18 +277,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -475,16 +632,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="160.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1">
@@ -508,19 +665,132 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
         <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="26">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -531,15 +801,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="9" max="9" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="81.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1">
@@ -578,6 +849,38 @@
       </c>
       <c r="I4" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="H5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="H6" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="H7" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="H8" t="s">
+        <v>53</v>
+      </c>
+      <c r="I8" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>